<commit_message>
Updates with Time average and tickets average
</commit_message>
<xml_diff>
--- a/static/RequestTimeAverage.xlsx
+++ b/static/RequestTimeAverage.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\syed.nusrath\Desktop\EY_Learning\Django\Charts\files\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B026F236-F226-4E72-813E-BAD2D68A1E2D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{97D6FE0B-AA71-49B2-8EDF-4AA658DB2DAD}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>name</t>
   </si>
@@ -38,19 +32,31 @@
     <t>value</t>
   </si>
   <si>
-    <t>Tasks</t>
-  </si>
-  <si>
-    <t>INC</t>
-  </si>
-  <si>
-    <t>ALL</t>
+    <t>Number of Managed:</t>
+  </si>
+  <si>
+    <t>Accounts:</t>
+  </si>
+  <si>
+    <t>Sales:</t>
+  </si>
+  <si>
+    <t>Licensed End users:</t>
+  </si>
+  <si>
+    <t>Average Time Open(Hrs) - Tasks</t>
+  </si>
+  <si>
+    <t>Average Time Open(Hrs) -  Incidents</t>
+  </si>
+  <si>
+    <t>Average Time Open(Hrs) - ALL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -142,7 +148,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -194,7 +200,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -388,23 +394,23 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56A7E37F-07C3-484F-A3C6-75075896CE7B}">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.77734375" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -417,7 +423,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B2">
         <v>68.849999999999994</v>
@@ -425,7 +431,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B3">
         <v>45.26</v>
@@ -433,10 +439,39 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B4">
         <v>66.040000000000006</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>130315</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>3709</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11">
+        <v>2161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>